<commit_message>
Update docs and report template
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steeven/GitHub/Jung/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0D39BC-E666-C647-B7C5-605AE4EE1032}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0B8841-CD5B-2949-8F7F-CD9273DF573C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{F6E1E2D4-B50E-0740-81F4-8B9EDC80F8FA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
     <sheet name="Graph" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Identify some third-party non-trivial distributed applications and analyze them</t>
   </si>
   <si>
-    <t xml:space="preserve">Write the report, prepare the poster and presentation </t>
-  </si>
-  <si>
     <t>Have a pizza</t>
   </si>
   <si>
@@ -103,12 +100,6 @@
     <t>Deadlines</t>
   </si>
   <si>
-    <t>07.Mar: Title and description</t>
-  </si>
-  <si>
-    <t>11. Apr: Progress report</t>
-  </si>
-  <si>
     <t>Develop a reader tool to "decrypt" the traces [non-essential]</t>
   </si>
   <si>
@@ -125,6 +116,33 @@
   </si>
   <si>
     <t>End week</t>
+  </si>
+  <si>
+    <t>25. Jun: final report</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>On hold</t>
+  </si>
+  <si>
+    <t>Write the report</t>
+  </si>
+  <si>
+    <t>07.Mar: Title and description (projectDescription.pdf)</t>
+  </si>
+  <si>
+    <t>11. Apr: Progress report (planningGraph.pdf)</t>
+  </si>
+  <si>
+    <t>30. May: Progress report (statusReport.pdf) and report draft</t>
   </si>
 </sst>
 </file>
@@ -268,7 +286,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Timeline!$D$2</c:f>
+              <c:f>Timeline!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -287,7 +305,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Timeline!$B$3:$C$18</c:f>
+              <c:f>Timeline!$B$3:$D$18</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -334,10 +352,60 @@
                     <c:v>Identify some third-party non-trivial distributed applications and analyze them</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Write the report, prepare the poster and presentation </c:v>
+                    <c:v>Write the report</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>Have a pizza</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>On hold</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>On hold</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>TODO</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>TODO</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>TODO</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -395,7 +463,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Timeline!$D$3:$D$18</c:f>
+              <c:f>Timeline!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -461,7 +529,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Timeline!$E$2</c:f>
+              <c:f>Timeline!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -482,7 +550,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Timeline!$B$3:$C$18</c:f>
+              <c:f>Timeline!$B$3:$D$18</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -529,10 +597,60 @@
                     <c:v>Identify some third-party non-trivial distributed applications and analyze them</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Write the report, prepare the poster and presentation </c:v>
+                    <c:v>Write the report</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>Have a pizza</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Done</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>On hold</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>On hold</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>TODO</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>TODO</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>TODO</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -590,7 +708,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Timeline!$E$3:$E$18</c:f>
+              <c:f>Timeline!$F$3:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1764,526 +1882,583 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9473EE3-CA3F-2146-A1E4-FA60DDD73597}">
-  <dimension ref="B2:K21"/>
+  <dimension ref="B2:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="96.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="6" customWidth="1"/>
-    <col min="5" max="6" width="13.1640625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="5" style="3" customWidth="1"/>
-    <col min="9" max="10" width="10.83203125" style="3"/>
-    <col min="11" max="11" width="50" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="3"/>
+    <col min="2" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="96.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="6" customWidth="1"/>
+    <col min="6" max="7" width="13.1640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="6.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="5" style="3" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" style="3"/>
+    <col min="12" max="12" width="66.33203125" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5">
+      <c r="E3" s="5">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="5">
-        <f>D3+E3</f>
+      <c r="G3" s="5">
+        <f>E3+F3</f>
         <v>1</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="7">
+      <c r="J3" s="7">
         <v>44242</v>
       </c>
-      <c r="J3" s="7">
+      <c r="K3" s="7">
         <v>44244</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5">
+      <c r="E4" s="5">
         <v>0</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="5">
-        <f t="shared" ref="F4:F18" si="0">D4+E4</f>
+      <c r="G4" s="5">
+        <f t="shared" ref="G4:G18" si="0">E4+F4</f>
         <v>1</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>1</v>
       </c>
-      <c r="I4" s="7">
+      <c r="J4" s="7">
         <v>44249</v>
       </c>
-      <c r="J4" s="7">
+      <c r="K4" s="7">
         <v>44251</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>2</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
         <v>44256</v>
       </c>
-      <c r="J5" s="7">
+      <c r="K5" s="7">
         <v>44258</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>22</v>
+      <c r="L5" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="5">
+        <v>29</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="4">
         <v>3</v>
       </c>
-      <c r="I6" s="7">
+      <c r="J6" s="7">
         <v>44263</v>
       </c>
-      <c r="J6" s="7">
+      <c r="K6" s="7">
         <v>44265</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5">
+      <c r="E7" s="5">
         <v>2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="4">
         <v>4</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="7">
         <v>44270</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="4"/>
+      <c r="K7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="5">
+      <c r="E8" s="5">
         <v>3</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>1</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <v>5</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="7">
         <v>44277</v>
       </c>
-      <c r="J8" s="7">
+      <c r="K8" s="7">
         <v>44281</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5">
+      <c r="E9" s="5">
         <v>3</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <v>6</v>
       </c>
-      <c r="I9" s="7">
+      <c r="J9" s="7">
         <v>44284</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="4"/>
+      <c r="K9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="5">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="5">
         <v>4</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="4">
         <v>7</v>
       </c>
-      <c r="I10" s="7">
+      <c r="J10" s="7">
         <v>44291</v>
       </c>
-      <c r="J10" s="7">
+      <c r="K10" s="7">
         <v>44295</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>23</v>
+      <c r="L10" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="5">
         <v>5</v>
       </c>
-      <c r="E11" s="5">
+      <c r="F11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="5">
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H11" s="4">
+      <c r="I11" s="4">
         <v>8</v>
       </c>
-      <c r="I11" s="7">
+      <c r="J11" s="7">
         <v>44298</v>
       </c>
-      <c r="J11" s="7">
+      <c r="K11" s="7">
         <v>44302</v>
       </c>
-      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="D12" s="5">
-        <v>5</v>
       </c>
       <c r="E12" s="5">
         <v>5</v>
       </c>
       <c r="F12" s="5">
+        <v>5</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H12" s="4">
+      <c r="I12" s="4">
         <v>9</v>
       </c>
-      <c r="I12" s="7">
+      <c r="J12" s="7">
         <v>44305</v>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="4"/>
+      <c r="K12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="5">
+      <c r="E13" s="5">
         <v>6</v>
       </c>
-      <c r="E13" s="5">
+      <c r="F13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" s="5">
+      <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="4">
         <v>10</v>
       </c>
-      <c r="I13" s="7">
+      <c r="J13" s="7">
         <v>44312</v>
       </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="K13" s="7">
+        <v>44314</v>
+      </c>
+      <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="5">
+        <v>31</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="5">
         <v>10</v>
       </c>
-      <c r="E14" s="5">
+      <c r="F14" s="5">
         <v>2</v>
       </c>
-      <c r="F14" s="5">
+      <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="4">
         <v>11</v>
       </c>
-      <c r="I14" s="7">
+      <c r="J14" s="7">
         <v>44319</v>
       </c>
-      <c r="J14" s="4"/>
       <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="5">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="5">
         <v>10</v>
       </c>
-      <c r="E15" s="5">
+      <c r="F15" s="5">
         <v>2</v>
       </c>
-      <c r="F15" s="5">
+      <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
         <v>12</v>
       </c>
-      <c r="I15" s="7">
+      <c r="J15" s="7">
         <v>44326</v>
       </c>
-      <c r="J15" s="4"/>
       <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="5">
+      <c r="E16" s="5">
         <v>13</v>
       </c>
-      <c r="E16" s="5">
+      <c r="F16" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="5">
+      <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H16" s="4">
+      <c r="I16" s="4">
         <v>13</v>
       </c>
-      <c r="I16" s="7">
+      <c r="J16" s="7">
         <v>44333</v>
       </c>
-      <c r="J16" s="4"/>
       <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="5">
+        <v>30</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="5">
         <v>11</v>
       </c>
-      <c r="E17" s="5">
+      <c r="F17" s="5">
         <v>3</v>
       </c>
-      <c r="F17" s="5">
+      <c r="G17" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H17" s="4">
+      <c r="I17" s="4">
         <v>14</v>
       </c>
-      <c r="I17" s="7">
+      <c r="J17" s="7">
         <v>44340</v>
       </c>
-      <c r="J17" s="4"/>
       <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="5">
+        <v>30</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="5">
         <v>14</v>
       </c>
-      <c r="E18" s="5">
+      <c r="F18" s="5">
         <v>1</v>
       </c>
-      <c r="F18" s="5">
+      <c r="G18" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H18" s="4">
+      <c r="I18" s="4">
         <v>15</v>
       </c>
-      <c r="I18" s="7">
+      <c r="J18" s="7">
         <v>44347</v>
       </c>
-      <c r="J18" s="4"/>
       <c r="K18" s="4"/>
+      <c r="L18" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H19" s="4">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I19" s="4">
         <v>16</v>
       </c>
-      <c r="I19" s="7">
+      <c r="J19" s="7">
         <v>44354</v>
       </c>
-      <c r="J19" s="4"/>
       <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H20" s="4">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I20" s="4">
         <v>17</v>
       </c>
-      <c r="I20" s="7">
+      <c r="J20" s="7">
         <v>44361</v>
       </c>
-      <c r="J20" s="4"/>
       <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H21" s="4">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I21" s="4">
         <v>18</v>
       </c>
-      <c r="I21" s="7">
+      <c r="J21" s="7">
         <v>44368</v>
       </c>
-      <c r="J21" s="4"/>
       <c r="K21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update docs, add pagefaults and docker-compose
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steeven/GitHub/Jung/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0B8841-CD5B-2949-8F7F-CD9273DF573C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DC1DF4-D786-7E44-9DF4-AD2FA39ACBCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{F6E1E2D4-B50E-0740-81F4-8B9EDC80F8FA}"/>
   </bookViews>
@@ -396,7 +396,7 @@
                     <c:v>On hold</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>On hold</c:v>
+                    <c:v>TODO</c:v>
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>TODO</c:v>
@@ -641,7 +641,7 @@
                     <c:v>On hold</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>On hold</c:v>
+                    <c:v>TODO</c:v>
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>TODO</c:v>
@@ -1885,7 +1885,7 @@
   <dimension ref="B2:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2303,7 +2303,9 @@
       <c r="J14" s="7">
         <v>44319</v>
       </c>
-      <c r="K14" s="4"/>
+      <c r="K14" s="7">
+        <v>44323</v>
+      </c>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -2311,7 +2313,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Add custom mutex and locks demo
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steeven/GitHub/Jung/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DC1DF4-D786-7E44-9DF4-AD2FA39ACBCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A020B84-F3DE-1345-820C-95A61512F955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{F6E1E2D4-B50E-0740-81F4-8B9EDC80F8FA}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="B2:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2334,7 +2334,9 @@
       <c r="J15" s="7">
         <v>44326</v>
       </c>
-      <c r="K15" s="4"/>
+      <c r="K15" s="7">
+        <v>44330</v>
+      </c>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Format code, update docs
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steeven/GitHub/Jung/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F2DE09-3543-3B4C-B8CE-9C10CB4C747E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B89B2C-AED0-1040-A3F6-F1812FEF7C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{F6E1E2D4-B50E-0740-81F4-8B9EDC80F8FA}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="B2:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2444,7 +2444,9 @@
       <c r="J19" s="7">
         <v>44354</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="7">
+        <v>44358</v>
+      </c>
       <c r="L19" s="4"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update docs and report
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steeven/GitHub/Jung/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B89B2C-AED0-1040-A3F6-F1812FEF7C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED89106-333F-534A-8B82-B33233F19459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{F6E1E2D4-B50E-0740-81F4-8B9EDC80F8FA}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="B2:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2456,7 +2456,9 @@
       <c r="J20" s="7">
         <v>44361</v>
       </c>
-      <c r="K20" s="4"/>
+      <c r="K20" s="7">
+        <v>44365</v>
+      </c>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add randomness to server
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steeven/GitHub/Jung/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED89106-333F-534A-8B82-B33233F19459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABE0B76-830F-A541-94B9-244AAFA607D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{F6E1E2D4-B50E-0740-81F4-8B9EDC80F8FA}"/>
   </bookViews>
@@ -399,7 +399,7 @@
                     <c:v>Dropped</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>Doing</c:v>
+                    <c:v>Done</c:v>
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>Dropped</c:v>
@@ -644,7 +644,7 @@
                     <c:v>Dropped</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>Doing</c:v>
+                    <c:v>Done</c:v>
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>Dropped</c:v>
@@ -1888,7 +1888,7 @@
   <dimension ref="B2:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2316,7 +2316,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>25</v>
@@ -2468,7 +2468,9 @@
       <c r="J21" s="7">
         <v>44368</v>
       </c>
-      <c r="K21" s="4"/>
+      <c r="K21" s="7">
+        <v>44370</v>
+      </c>
       <c r="L21" s="4" t="s">
         <v>34</v>
       </c>

</xml_diff>